<commit_message>
add alexnet, resnet18 unfinished
</commit_message>
<xml_diff>
--- a/total_result.xlsx
+++ b/total_result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyb\Documents\NetSarang Computer\6\Xftp\Temporary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40338CCF-0596-4DC5-B7C4-EAF7DF8D4CDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C666A3-102B-4D4D-927B-5DC93E904AB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -500,10 +500,18 @@
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="3">
+        <v>0.61180000000000001</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.82920000000000005</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.60570000000000002</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.8236</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">

</xml_diff>

<commit_message>
cambricon quantify result, test time result
</commit_message>
<xml_diff>
--- a/total_result.xlsx
+++ b/total_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyb\Documents\NetSarang Computer\6\Xftp\Temporary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e4c124f38714c139/文档/NetSarang Computer/6/Xftp/Temporary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C666A3-102B-4D4D-927B-5DC93E904AB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{02B032D2-6C20-4B08-9E99-ABFD1269EA97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{52FB85F6-B1B6-4C1A-9F69-103E84AAF2FA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>lenet5</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,6 +66,122 @@
   </si>
   <si>
     <t>top5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始精度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寒武纪量化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cpu-full</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mlu-8bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fold-bn-mlu-8bit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>imgnet-50batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>722.7472879886627</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24.685790061950684</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>49.80574893951416</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.992085933685303</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cifarnet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>85.71440982818604</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.424906969070435</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vgg64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>531.0056591033936</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.820096015930176</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resnet18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1517.6351280212402</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36.85030388832092</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>36.40901303291321</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resnet50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>62.62694787979126</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>53.05603790283203</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5381.475935935974</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -97,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -120,11 +236,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -133,7 +275,34 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -416,19 +585,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="19.25" customWidth="1"/>
+    <col min="1" max="5" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -436,8 +604,16 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,8 +623,16 @@
       <c r="C2" s="3">
         <v>0.9929</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="11">
+        <v>0.99409999999999998</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="11">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -458,8 +642,16 @@
       <c r="C3" s="3">
         <v>0.81910000000000005</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="9">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9">
+        <v>0.81079999999999997</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -469,20 +661,40 @@
       <c r="C4" s="3">
         <v>0.92559999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+      <c r="F4" s="9">
+        <v>0.92859999999999998</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="9">
+        <v>0.92349999999999999</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
+      <c r="E6" s="10"/>
+      <c r="H6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -495,8 +707,24 @@
       <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -512,8 +740,24 @@
       <c r="E8" s="3">
         <v>0.8236</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H8" s="8">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9">
+        <v>0.82179999999999997</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="9">
+        <v>0.57189999999999996</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="9">
+        <v>0.79339999999999999</v>
+      </c>
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -521,12 +765,169 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="26">
+    <mergeCell ref="C15:E15"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="L6:O6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>